<commit_message>
tambahain pengecekan  data import KPKP
</commit_message>
<xml_diff>
--- a/import/kpkp/data-kpkp per Januari 2024.xlsx
+++ b/import/kpkp/data-kpkp per Januari 2024.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New folder\GKP\Pnt\Pemutakhiran\DATA KPKP-20240113T034056Z-001\DATA KPKP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sisfo_kamsaw\import\kpkp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2E8BB7-BA4A-4155-875C-D22A3092891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -887,9 +897,6 @@
     <t>ANAK AGUNG AYU PANJI VIRALAKSMI</t>
   </si>
   <si>
-    <t>ANDREAS WIJAYA</t>
-  </si>
-  <si>
     <t>ANDRIE SUPARDI</t>
   </si>
   <si>
@@ -929,9 +936,6 @@
     <t>ERLIANA BANYUTAWA</t>
   </si>
   <si>
-    <t>FREDY  TUMBELAKA</t>
-  </si>
-  <si>
     <t>GUNANSI</t>
   </si>
   <si>
@@ -992,9 +996,6 @@
     <t>MATILLE SUPIATI MARPAUNG</t>
   </si>
   <si>
-    <t>MARYANTA SAIRIN</t>
-  </si>
-  <si>
     <t>MURNIJANTI RIKIN</t>
   </si>
   <si>
@@ -1740,12 +1741,21 @@
   </si>
   <si>
     <t>TASEM</t>
+  </si>
+  <si>
+    <t>ANDREAS</t>
+  </si>
+  <si>
+    <t>FREDY TUMBELAKA</t>
+  </si>
+  <si>
+    <t>MIRYANTA SAIRIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ yyyy"/>
   </numFmts>
@@ -1812,24 +1822,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2104,11 +2097,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J603"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A555" workbookViewId="0">
-      <selection activeCell="B563" sqref="B563"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11025,7 +11018,7 @@
         <v>278</v>
       </c>
       <c r="B279" t="s">
-        <v>287</v>
+        <v>569</v>
       </c>
       <c r="C279">
         <v>2</v>
@@ -11057,7 +11050,7 @@
         <v>279</v>
       </c>
       <c r="B280" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C280">
         <v>2</v>
@@ -11089,7 +11082,7 @@
         <v>280</v>
       </c>
       <c r="B281" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C281">
         <v>3</v>
@@ -11121,7 +11114,7 @@
         <v>281</v>
       </c>
       <c r="B282" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C282">
         <v>4</v>
@@ -11153,7 +11146,7 @@
         <v>282</v>
       </c>
       <c r="B283" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C283">
         <v>1</v>
@@ -11185,7 +11178,7 @@
         <v>283</v>
       </c>
       <c r="B284" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C284">
         <v>4</v>
@@ -11217,7 +11210,7 @@
         <v>284</v>
       </c>
       <c r="B285" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C285">
         <v>3</v>
@@ -11249,7 +11242,7 @@
         <v>285</v>
       </c>
       <c r="B286" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C286">
         <v>3</v>
@@ -11281,7 +11274,7 @@
         <v>286</v>
       </c>
       <c r="B287" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C287">
         <v>4</v>
@@ -11313,7 +11306,7 @@
         <v>287</v>
       </c>
       <c r="B288" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C288">
         <v>5</v>
@@ -11345,7 +11338,7 @@
         <v>288</v>
       </c>
       <c r="B289" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C289">
         <v>1</v>
@@ -11377,7 +11370,7 @@
         <v>289</v>
       </c>
       <c r="B290" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C290">
         <v>4</v>
@@ -11409,7 +11402,7 @@
         <v>290</v>
       </c>
       <c r="B291" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C291">
         <v>4</v>
@@ -11441,7 +11434,7 @@
         <v>291</v>
       </c>
       <c r="B292" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C292">
         <v>1</v>
@@ -11473,7 +11466,7 @@
         <v>292</v>
       </c>
       <c r="B293" t="s">
-        <v>301</v>
+        <v>570</v>
       </c>
       <c r="C293">
         <v>3</v>
@@ -11505,7 +11498,7 @@
         <v>293</v>
       </c>
       <c r="B294" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C294">
         <v>3</v>
@@ -11537,7 +11530,7 @@
         <v>294</v>
       </c>
       <c r="B295" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C295">
         <v>5</v>
@@ -11569,7 +11562,7 @@
         <v>295</v>
       </c>
       <c r="B296" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C296">
         <v>5</v>
@@ -11601,7 +11594,7 @@
         <v>296</v>
       </c>
       <c r="B297" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C297">
         <v>2</v>
@@ -11633,7 +11626,7 @@
         <v>297</v>
       </c>
       <c r="B298" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C298">
         <v>2</v>
@@ -11665,7 +11658,7 @@
         <v>298</v>
       </c>
       <c r="B299" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C299">
         <v>1</v>
@@ -11697,7 +11690,7 @@
         <v>299</v>
       </c>
       <c r="B300" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C300">
         <v>2</v>
@@ -11729,7 +11722,7 @@
         <v>300</v>
       </c>
       <c r="B301" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C301">
         <v>3</v>
@@ -11761,7 +11754,7 @@
         <v>301</v>
       </c>
       <c r="B302" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C302">
         <v>3</v>
@@ -11793,7 +11786,7 @@
         <v>302</v>
       </c>
       <c r="B303" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C303">
         <v>4</v>
@@ -11825,7 +11818,7 @@
         <v>303</v>
       </c>
       <c r="B304" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C304">
         <v>4</v>
@@ -11857,7 +11850,7 @@
         <v>304</v>
       </c>
       <c r="B305" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C305">
         <v>3</v>
@@ -11889,7 +11882,7 @@
         <v>305</v>
       </c>
       <c r="B306" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C306">
         <v>2</v>
@@ -11921,7 +11914,7 @@
         <v>306</v>
       </c>
       <c r="B307" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C307">
         <v>1</v>
@@ -11953,7 +11946,7 @@
         <v>307</v>
       </c>
       <c r="B308" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C308">
         <v>4</v>
@@ -11985,7 +11978,7 @@
         <v>308</v>
       </c>
       <c r="B309" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C309">
         <v>2</v>
@@ -12017,7 +12010,7 @@
         <v>309</v>
       </c>
       <c r="B310" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C310">
         <v>4</v>
@@ -12049,7 +12042,7 @@
         <v>310</v>
       </c>
       <c r="B311" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C311">
         <v>1</v>
@@ -12081,7 +12074,7 @@
         <v>311</v>
       </c>
       <c r="B312" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C312">
         <v>1</v>
@@ -12113,7 +12106,7 @@
         <v>312</v>
       </c>
       <c r="B313" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C313">
         <v>1</v>
@@ -12145,7 +12138,7 @@
         <v>313</v>
       </c>
       <c r="B314" t="s">
-        <v>322</v>
+        <v>571</v>
       </c>
       <c r="C314">
         <v>1</v>
@@ -12177,7 +12170,7 @@
         <v>314</v>
       </c>
       <c r="B315" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C315">
         <v>2</v>
@@ -12209,7 +12202,7 @@
         <v>315</v>
       </c>
       <c r="B316" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C316">
         <v>4</v>
@@ -12241,7 +12234,7 @@
         <v>316</v>
       </c>
       <c r="B317" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C317">
         <v>3</v>
@@ -12273,7 +12266,7 @@
         <v>317</v>
       </c>
       <c r="B318" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C318">
         <v>4</v>
@@ -12305,7 +12298,7 @@
         <v>318</v>
       </c>
       <c r="B319" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C319">
         <v>4</v>
@@ -12337,7 +12330,7 @@
         <v>319</v>
       </c>
       <c r="B320" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C320">
         <v>2</v>
@@ -12369,7 +12362,7 @@
         <v>320</v>
       </c>
       <c r="B321" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C321">
         <v>4</v>
@@ -12401,7 +12394,7 @@
         <v>321</v>
       </c>
       <c r="B322" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C322">
         <v>1</v>
@@ -12433,7 +12426,7 @@
         <v>322</v>
       </c>
       <c r="B323" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C323">
         <v>1</v>
@@ -12465,7 +12458,7 @@
         <v>323</v>
       </c>
       <c r="B324" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C324">
         <v>5</v>
@@ -12497,7 +12490,7 @@
         <v>324</v>
       </c>
       <c r="B325" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C325">
         <v>5</v>
@@ -12529,7 +12522,7 @@
         <v>325</v>
       </c>
       <c r="B326" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C326">
         <v>4</v>
@@ -12561,7 +12554,7 @@
         <v>326</v>
       </c>
       <c r="B327" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C327">
         <v>2</v>
@@ -12593,7 +12586,7 @@
         <v>327</v>
       </c>
       <c r="B328" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C328">
         <v>2</v>
@@ -12625,7 +12618,7 @@
         <v>328</v>
       </c>
       <c r="B329" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C329">
         <v>1</v>
@@ -12657,7 +12650,7 @@
         <v>329</v>
       </c>
       <c r="B330" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C330">
         <v>3</v>
@@ -12689,7 +12682,7 @@
         <v>330</v>
       </c>
       <c r="B331" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C331">
         <v>3</v>
@@ -12721,7 +12714,7 @@
         <v>331</v>
       </c>
       <c r="B332" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C332">
         <v>2</v>
@@ -12753,7 +12746,7 @@
         <v>332</v>
       </c>
       <c r="B333" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C333">
         <v>2</v>
@@ -12785,7 +12778,7 @@
         <v>333</v>
       </c>
       <c r="B334" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C334">
         <v>4</v>
@@ -12817,7 +12810,7 @@
         <v>334</v>
       </c>
       <c r="B335" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C335">
         <v>3</v>
@@ -12849,7 +12842,7 @@
         <v>335</v>
       </c>
       <c r="B336" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C336">
         <v>2</v>
@@ -12881,7 +12874,7 @@
         <v>336</v>
       </c>
       <c r="B337" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C337">
         <v>1</v>
@@ -12913,7 +12906,7 @@
         <v>337</v>
       </c>
       <c r="B338" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C338">
         <v>5</v>
@@ -12945,7 +12938,7 @@
         <v>338</v>
       </c>
       <c r="B339" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C339">
         <v>5</v>
@@ -12977,7 +12970,7 @@
         <v>339</v>
       </c>
       <c r="B340" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C340">
         <v>1</v>
@@ -13009,7 +13002,7 @@
         <v>340</v>
       </c>
       <c r="B341" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C341">
         <v>2</v>
@@ -13041,7 +13034,7 @@
         <v>341</v>
       </c>
       <c r="B342" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C342">
         <v>4</v>
@@ -13073,7 +13066,7 @@
         <v>342</v>
       </c>
       <c r="B343" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C343">
         <v>2</v>
@@ -13105,7 +13098,7 @@
         <v>343</v>
       </c>
       <c r="B344" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C344">
         <v>2</v>
@@ -13137,7 +13130,7 @@
         <v>344</v>
       </c>
       <c r="B345" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C345">
         <v>3</v>
@@ -13169,7 +13162,7 @@
         <v>345</v>
       </c>
       <c r="B346" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C346">
         <v>4</v>
@@ -13201,7 +13194,7 @@
         <v>346</v>
       </c>
       <c r="B347" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C347">
         <v>1</v>
@@ -13233,7 +13226,7 @@
         <v>347</v>
       </c>
       <c r="B348" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C348">
         <v>5</v>
@@ -13265,7 +13258,7 @@
         <v>348</v>
       </c>
       <c r="B349" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C349">
         <v>3</v>
@@ -13297,7 +13290,7 @@
         <v>349</v>
       </c>
       <c r="B350" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C350">
         <v>4</v>
@@ -13329,7 +13322,7 @@
         <v>350</v>
       </c>
       <c r="B351" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C351">
         <v>1</v>
@@ -13361,7 +13354,7 @@
         <v>351</v>
       </c>
       <c r="B352" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C352">
         <v>2</v>
@@ -13393,7 +13386,7 @@
         <v>352</v>
       </c>
       <c r="B353" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C353">
         <v>2</v>
@@ -13425,7 +13418,7 @@
         <v>353</v>
       </c>
       <c r="B354" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C354">
         <v>3</v>
@@ -13457,7 +13450,7 @@
         <v>354</v>
       </c>
       <c r="B355" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C355">
         <v>5</v>
@@ -13489,7 +13482,7 @@
         <v>355</v>
       </c>
       <c r="B356" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C356">
         <v>1</v>
@@ -13521,7 +13514,7 @@
         <v>356</v>
       </c>
       <c r="B357" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C357">
         <v>1</v>
@@ -13553,7 +13546,7 @@
         <v>357</v>
       </c>
       <c r="B358" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C358">
         <v>3</v>
@@ -13585,7 +13578,7 @@
         <v>358</v>
       </c>
       <c r="B359" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C359">
         <v>1</v>
@@ -13617,7 +13610,7 @@
         <v>359</v>
       </c>
       <c r="B360" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C360">
         <v>1</v>
@@ -13649,7 +13642,7 @@
         <v>360</v>
       </c>
       <c r="B361" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C361">
         <v>1</v>
@@ -13681,7 +13674,7 @@
         <v>361</v>
       </c>
       <c r="B362" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C362">
         <v>3</v>
@@ -13713,7 +13706,7 @@
         <v>362</v>
       </c>
       <c r="B363" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C363">
         <v>1</v>
@@ -13745,7 +13738,7 @@
         <v>363</v>
       </c>
       <c r="B364" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C364">
         <v>4</v>
@@ -13777,7 +13770,7 @@
         <v>364</v>
       </c>
       <c r="B365" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C365">
         <v>5</v>
@@ -13809,7 +13802,7 @@
         <v>365</v>
       </c>
       <c r="B366" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C366">
         <v>3</v>
@@ -13841,7 +13834,7 @@
         <v>366</v>
       </c>
       <c r="B367" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C367">
         <v>5</v>
@@ -13873,7 +13866,7 @@
         <v>367</v>
       </c>
       <c r="B368" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C368">
         <v>2</v>
@@ -13905,7 +13898,7 @@
         <v>368</v>
       </c>
       <c r="B369" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C369">
         <v>1</v>
@@ -13937,7 +13930,7 @@
         <v>369</v>
       </c>
       <c r="B370" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C370">
         <v>4</v>
@@ -13969,7 +13962,7 @@
         <v>370</v>
       </c>
       <c r="B371" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C371">
         <v>1</v>
@@ -14001,7 +13994,7 @@
         <v>371</v>
       </c>
       <c r="B372" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C372">
         <v>2</v>
@@ -14033,7 +14026,7 @@
         <v>372</v>
       </c>
       <c r="B373" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C373">
         <v>2</v>
@@ -14065,7 +14058,7 @@
         <v>373</v>
       </c>
       <c r="B374" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C374">
         <v>2</v>
@@ -14097,7 +14090,7 @@
         <v>374</v>
       </c>
       <c r="B375" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C375">
         <v>3</v>
@@ -14129,7 +14122,7 @@
         <v>375</v>
       </c>
       <c r="B376" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C376">
         <v>2</v>
@@ -14161,7 +14154,7 @@
         <v>376</v>
       </c>
       <c r="B377" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C377">
         <v>4</v>
@@ -14193,7 +14186,7 @@
         <v>377</v>
       </c>
       <c r="B378" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C378">
         <v>3</v>
@@ -14225,7 +14218,7 @@
         <v>378</v>
       </c>
       <c r="B379" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C379">
         <v>1</v>
@@ -14257,7 +14250,7 @@
         <v>379</v>
       </c>
       <c r="B380" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C380">
         <v>4</v>
@@ -14289,7 +14282,7 @@
         <v>380</v>
       </c>
       <c r="B381" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C381">
         <v>4</v>
@@ -14321,7 +14314,7 @@
         <v>381</v>
       </c>
       <c r="B382" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C382">
         <v>1</v>
@@ -14353,7 +14346,7 @@
         <v>382</v>
       </c>
       <c r="B383" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C383">
         <v>3</v>
@@ -14385,7 +14378,7 @@
         <v>383</v>
       </c>
       <c r="B384" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C384">
         <v>4</v>
@@ -14417,7 +14410,7 @@
         <v>384</v>
       </c>
       <c r="B385" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C385">
         <v>2</v>
@@ -14449,7 +14442,7 @@
         <v>385</v>
       </c>
       <c r="B386" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C386">
         <v>2</v>
@@ -14481,7 +14474,7 @@
         <v>386</v>
       </c>
       <c r="B387" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C387">
         <v>4</v>
@@ -14513,7 +14506,7 @@
         <v>387</v>
       </c>
       <c r="B388" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C388">
         <v>3</v>
@@ -14545,7 +14538,7 @@
         <v>388</v>
       </c>
       <c r="B389" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C389">
         <v>1</v>
@@ -14577,7 +14570,7 @@
         <v>389</v>
       </c>
       <c r="B390" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C390">
         <v>1</v>
@@ -14609,7 +14602,7 @@
         <v>390</v>
       </c>
       <c r="B391" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C391">
         <v>3</v>
@@ -14641,7 +14634,7 @@
         <v>391</v>
       </c>
       <c r="B392" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C392">
         <v>2</v>
@@ -14673,7 +14666,7 @@
         <v>392</v>
       </c>
       <c r="B393" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C393">
         <v>2</v>
@@ -14705,7 +14698,7 @@
         <v>393</v>
       </c>
       <c r="B394" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C394">
         <v>4</v>
@@ -14737,7 +14730,7 @@
         <v>394</v>
       </c>
       <c r="B395" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C395">
         <v>2</v>
@@ -14769,7 +14762,7 @@
         <v>395</v>
       </c>
       <c r="B396" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C396">
         <v>2</v>
@@ -14801,7 +14794,7 @@
         <v>396</v>
       </c>
       <c r="B397" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C397">
         <v>2</v>
@@ -14833,7 +14826,7 @@
         <v>397</v>
       </c>
       <c r="B398" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C398">
         <v>3</v>
@@ -14865,7 +14858,7 @@
         <v>398</v>
       </c>
       <c r="B399" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C399">
         <v>1</v>
@@ -14897,7 +14890,7 @@
         <v>399</v>
       </c>
       <c r="B400" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C400">
         <v>1</v>
@@ -14929,7 +14922,7 @@
         <v>400</v>
       </c>
       <c r="B401" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C401">
         <v>2</v>
@@ -14961,7 +14954,7 @@
         <v>401</v>
       </c>
       <c r="B402" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C402">
         <v>2</v>
@@ -14993,7 +14986,7 @@
         <v>402</v>
       </c>
       <c r="B403" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C403">
         <v>3</v>
@@ -15025,7 +15018,7 @@
         <v>403</v>
       </c>
       <c r="B404" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C404">
         <v>3</v>
@@ -15057,7 +15050,7 @@
         <v>404</v>
       </c>
       <c r="B405" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C405">
         <v>1</v>
@@ -15089,7 +15082,7 @@
         <v>405</v>
       </c>
       <c r="B406" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C406">
         <v>3</v>
@@ -15121,7 +15114,7 @@
         <v>406</v>
       </c>
       <c r="B407" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C407">
         <v>4</v>
@@ -15153,7 +15146,7 @@
         <v>407</v>
       </c>
       <c r="B408" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C408">
         <v>5</v>
@@ -15185,7 +15178,7 @@
         <v>408</v>
       </c>
       <c r="B409" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C409">
         <v>2</v>
@@ -15217,7 +15210,7 @@
         <v>409</v>
       </c>
       <c r="B410" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C410">
         <v>4</v>
@@ -15249,7 +15242,7 @@
         <v>410</v>
       </c>
       <c r="B411" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C411">
         <v>3</v>
@@ -15281,7 +15274,7 @@
         <v>411</v>
       </c>
       <c r="B412" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C412">
         <v>2</v>
@@ -15313,7 +15306,7 @@
         <v>412</v>
       </c>
       <c r="B413" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C413">
         <v>4</v>
@@ -15345,7 +15338,7 @@
         <v>413</v>
       </c>
       <c r="B414" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C414">
         <v>2</v>
@@ -15377,7 +15370,7 @@
         <v>414</v>
       </c>
       <c r="B415" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C415">
         <v>5</v>
@@ -15409,7 +15402,7 @@
         <v>415</v>
       </c>
       <c r="B416" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C416">
         <v>1</v>
@@ -15441,7 +15434,7 @@
         <v>416</v>
       </c>
       <c r="B417" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C417">
         <v>3</v>
@@ -15473,7 +15466,7 @@
         <v>417</v>
       </c>
       <c r="B418" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C418">
         <v>3</v>
@@ -15505,7 +15498,7 @@
         <v>418</v>
       </c>
       <c r="B419" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C419">
         <v>2</v>
@@ -15537,7 +15530,7 @@
         <v>419</v>
       </c>
       <c r="B420" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C420">
         <v>2</v>
@@ -15569,7 +15562,7 @@
         <v>420</v>
       </c>
       <c r="B421" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C421">
         <v>5</v>
@@ -15601,7 +15594,7 @@
         <v>421</v>
       </c>
       <c r="B422" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C422">
         <v>1</v>
@@ -15633,7 +15626,7 @@
         <v>422</v>
       </c>
       <c r="B423" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C423">
         <v>3</v>
@@ -15665,7 +15658,7 @@
         <v>423</v>
       </c>
       <c r="B424" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C424">
         <v>3</v>
@@ -15697,7 +15690,7 @@
         <v>424</v>
       </c>
       <c r="B425" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C425">
         <v>3</v>
@@ -15729,7 +15722,7 @@
         <v>425</v>
       </c>
       <c r="B426" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C426">
         <v>3</v>
@@ -15761,7 +15754,7 @@
         <v>426</v>
       </c>
       <c r="B427" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C427">
         <v>2</v>
@@ -15793,7 +15786,7 @@
         <v>427</v>
       </c>
       <c r="B428" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C428">
         <v>2</v>
@@ -15825,7 +15818,7 @@
         <v>428</v>
       </c>
       <c r="B429" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C429">
         <v>5</v>
@@ -15857,7 +15850,7 @@
         <v>429</v>
       </c>
       <c r="B430" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C430">
         <v>2</v>
@@ -15889,7 +15882,7 @@
         <v>430</v>
       </c>
       <c r="B431" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C431">
         <v>2</v>
@@ -15921,7 +15914,7 @@
         <v>431</v>
       </c>
       <c r="B432" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C432">
         <v>3</v>
@@ -15953,7 +15946,7 @@
         <v>432</v>
       </c>
       <c r="B433" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C433">
         <v>1</v>
@@ -15985,7 +15978,7 @@
         <v>433</v>
       </c>
       <c r="B434" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C434">
         <v>3</v>
@@ -16017,7 +16010,7 @@
         <v>434</v>
       </c>
       <c r="B435" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C435">
         <v>4</v>
@@ -16049,7 +16042,7 @@
         <v>435</v>
       </c>
       <c r="B436" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C436">
         <v>1</v>
@@ -16081,7 +16074,7 @@
         <v>436</v>
       </c>
       <c r="B437" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C437">
         <v>5</v>
@@ -16113,7 +16106,7 @@
         <v>437</v>
       </c>
       <c r="B438" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C438">
         <v>2</v>
@@ -16145,7 +16138,7 @@
         <v>438</v>
       </c>
       <c r="B439" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C439">
         <v>4</v>
@@ -16177,7 +16170,7 @@
         <v>439</v>
       </c>
       <c r="B440" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C440">
         <v>4</v>
@@ -16209,7 +16202,7 @@
         <v>440</v>
       </c>
       <c r="B441" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C441">
         <v>3</v>
@@ -16241,7 +16234,7 @@
         <v>441</v>
       </c>
       <c r="B442" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C442">
         <v>4</v>
@@ -16273,7 +16266,7 @@
         <v>442</v>
       </c>
       <c r="B443" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C443">
         <v>5</v>
@@ -16305,7 +16298,7 @@
         <v>443</v>
       </c>
       <c r="B444" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C444">
         <v>1</v>
@@ -16337,7 +16330,7 @@
         <v>444</v>
       </c>
       <c r="B445" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C445">
         <v>4</v>
@@ -16369,7 +16362,7 @@
         <v>445</v>
       </c>
       <c r="B446" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C446">
         <v>2</v>
@@ -16401,7 +16394,7 @@
         <v>446</v>
       </c>
       <c r="B447" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C447">
         <v>3</v>
@@ -16433,7 +16426,7 @@
         <v>447</v>
       </c>
       <c r="B448" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C448">
         <v>3</v>
@@ -16465,7 +16458,7 @@
         <v>448</v>
       </c>
       <c r="B449" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C449">
         <v>4</v>
@@ -16497,7 +16490,7 @@
         <v>449</v>
       </c>
       <c r="B450" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C450">
         <v>4</v>
@@ -16529,7 +16522,7 @@
         <v>450</v>
       </c>
       <c r="B451" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C451">
         <v>4</v>
@@ -16561,7 +16554,7 @@
         <v>451</v>
       </c>
       <c r="B452" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C452">
         <v>3</v>
@@ -16593,7 +16586,7 @@
         <v>452</v>
       </c>
       <c r="B453" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C453">
         <v>3</v>
@@ -16625,7 +16618,7 @@
         <v>453</v>
       </c>
       <c r="B454" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C454">
         <v>2</v>
@@ -16657,7 +16650,7 @@
         <v>454</v>
       </c>
       <c r="B455" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C455">
         <v>2</v>
@@ -16689,7 +16682,7 @@
         <v>455</v>
       </c>
       <c r="B456" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C456">
         <v>2</v>
@@ -16721,7 +16714,7 @@
         <v>456</v>
       </c>
       <c r="B457" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C457">
         <v>3</v>
@@ -16753,7 +16746,7 @@
         <v>457</v>
       </c>
       <c r="B458" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C458">
         <v>4</v>
@@ -16785,7 +16778,7 @@
         <v>458</v>
       </c>
       <c r="B459" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C459">
         <v>4</v>
@@ -16817,7 +16810,7 @@
         <v>459</v>
       </c>
       <c r="B460" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C460">
         <v>2</v>
@@ -16849,7 +16842,7 @@
         <v>460</v>
       </c>
       <c r="B461" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C461">
         <v>4</v>
@@ -16881,7 +16874,7 @@
         <v>461</v>
       </c>
       <c r="B462" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C462">
         <v>3</v>
@@ -16913,7 +16906,7 @@
         <v>462</v>
       </c>
       <c r="B463" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C463">
         <v>1</v>
@@ -16945,7 +16938,7 @@
         <v>463</v>
       </c>
       <c r="B464" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C464">
         <v>2</v>
@@ -16977,7 +16970,7 @@
         <v>464</v>
       </c>
       <c r="B465" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C465">
         <v>2</v>
@@ -17009,7 +17002,7 @@
         <v>465</v>
       </c>
       <c r="B466" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C466">
         <v>5</v>
@@ -17041,7 +17034,7 @@
         <v>466</v>
       </c>
       <c r="B467" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C467">
         <v>2</v>
@@ -17073,7 +17066,7 @@
         <v>467</v>
       </c>
       <c r="B468" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C468">
         <v>1</v>
@@ -17105,7 +17098,7 @@
         <v>468</v>
       </c>
       <c r="B469" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C469">
         <v>2</v>
@@ -17137,7 +17130,7 @@
         <v>469</v>
       </c>
       <c r="B470" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C470">
         <v>5</v>
@@ -17169,7 +17162,7 @@
         <v>470</v>
       </c>
       <c r="B471" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C471">
         <v>3</v>
@@ -17201,7 +17194,7 @@
         <v>471</v>
       </c>
       <c r="B472" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C472">
         <v>2</v>
@@ -17233,7 +17226,7 @@
         <v>472</v>
       </c>
       <c r="B473" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C473">
         <v>1</v>
@@ -17265,7 +17258,7 @@
         <v>473</v>
       </c>
       <c r="B474" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C474">
         <v>1</v>
@@ -17297,7 +17290,7 @@
         <v>474</v>
       </c>
       <c r="B475" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C475">
         <v>1</v>
@@ -17329,7 +17322,7 @@
         <v>475</v>
       </c>
       <c r="B476" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C476">
         <v>3</v>
@@ -17361,7 +17354,7 @@
         <v>476</v>
       </c>
       <c r="B477" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C477">
         <v>1</v>
@@ -17393,7 +17386,7 @@
         <v>477</v>
       </c>
       <c r="B478" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C478">
         <v>6</v>
@@ -17425,7 +17418,7 @@
         <v>478</v>
       </c>
       <c r="B479" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C479">
         <v>1</v>
@@ -17457,7 +17450,7 @@
         <v>479</v>
       </c>
       <c r="B480" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C480">
         <v>1</v>
@@ -17489,7 +17482,7 @@
         <v>480</v>
       </c>
       <c r="B481" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C481">
         <v>1</v>
@@ -17521,7 +17514,7 @@
         <v>481</v>
       </c>
       <c r="B482" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C482">
         <v>3</v>
@@ -17553,7 +17546,7 @@
         <v>482</v>
       </c>
       <c r="B483" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C483">
         <v>4</v>
@@ -17585,7 +17578,7 @@
         <v>483</v>
       </c>
       <c r="B484" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C484">
         <v>3</v>
@@ -17617,7 +17610,7 @@
         <v>484</v>
       </c>
       <c r="B485" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C485">
         <v>2</v>
@@ -17649,7 +17642,7 @@
         <v>485</v>
       </c>
       <c r="B486" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C486">
         <v>4</v>
@@ -17681,7 +17674,7 @@
         <v>486</v>
       </c>
       <c r="B487" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C487">
         <v>4</v>
@@ -17713,7 +17706,7 @@
         <v>487</v>
       </c>
       <c r="B488" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C488">
         <v>4</v>
@@ -17745,7 +17738,7 @@
         <v>488</v>
       </c>
       <c r="B489" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C489">
         <v>5</v>
@@ -17777,7 +17770,7 @@
         <v>489</v>
       </c>
       <c r="B490" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C490">
         <v>2</v>
@@ -17809,7 +17802,7 @@
         <v>490</v>
       </c>
       <c r="B491" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C491">
         <v>5</v>
@@ -17841,7 +17834,7 @@
         <v>491</v>
       </c>
       <c r="B492" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="C492">
         <v>1</v>
@@ -17873,7 +17866,7 @@
         <v>492</v>
       </c>
       <c r="B493" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C493">
         <v>2</v>
@@ -17905,7 +17898,7 @@
         <v>493</v>
       </c>
       <c r="B494" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C494">
         <v>4</v>
@@ -17937,7 +17930,7 @@
         <v>494</v>
       </c>
       <c r="B495" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C495">
         <v>3</v>
@@ -17969,7 +17962,7 @@
         <v>495</v>
       </c>
       <c r="B496" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C496">
         <v>4</v>
@@ -18001,7 +17994,7 @@
         <v>496</v>
       </c>
       <c r="B497" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C497">
         <v>4</v>
@@ -18033,7 +18026,7 @@
         <v>497</v>
       </c>
       <c r="B498" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C498">
         <v>6</v>
@@ -18065,7 +18058,7 @@
         <v>498</v>
       </c>
       <c r="B499" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C499">
         <v>3</v>
@@ -18097,7 +18090,7 @@
         <v>499</v>
       </c>
       <c r="B500" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C500">
         <v>1</v>
@@ -18129,7 +18122,7 @@
         <v>500</v>
       </c>
       <c r="B501" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C501">
         <v>3</v>
@@ -18161,7 +18154,7 @@
         <v>501</v>
       </c>
       <c r="B502" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C502">
         <v>3</v>
@@ -18193,7 +18186,7 @@
         <v>502</v>
       </c>
       <c r="B503" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C503">
         <v>3</v>
@@ -18225,7 +18218,7 @@
         <v>503</v>
       </c>
       <c r="B504" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C504">
         <v>2</v>
@@ -18257,7 +18250,7 @@
         <v>504</v>
       </c>
       <c r="B505" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C505">
         <v>3</v>
@@ -18289,7 +18282,7 @@
         <v>505</v>
       </c>
       <c r="B506" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C506">
         <v>5</v>
@@ -18321,7 +18314,7 @@
         <v>506</v>
       </c>
       <c r="B507" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C507">
         <v>3</v>
@@ -18353,7 +18346,7 @@
         <v>507</v>
       </c>
       <c r="B508" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C508">
         <v>3</v>
@@ -18385,7 +18378,7 @@
         <v>508</v>
       </c>
       <c r="B509" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C509">
         <v>5</v>
@@ -18417,7 +18410,7 @@
         <v>509</v>
       </c>
       <c r="B510" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C510">
         <v>3</v>
@@ -18449,7 +18442,7 @@
         <v>510</v>
       </c>
       <c r="B511" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C511">
         <v>4</v>
@@ -18481,7 +18474,7 @@
         <v>511</v>
       </c>
       <c r="B512" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C512">
         <v>1</v>
@@ -18513,7 +18506,7 @@
         <v>512</v>
       </c>
       <c r="B513" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C513">
         <v>2</v>
@@ -18545,7 +18538,7 @@
         <v>513</v>
       </c>
       <c r="B514" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C514">
         <v>3</v>
@@ -18577,7 +18570,7 @@
         <v>514</v>
       </c>
       <c r="B515" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C515">
         <v>2</v>
@@ -18609,7 +18602,7 @@
         <v>515</v>
       </c>
       <c r="B516" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C516">
         <v>2</v>
@@ -18641,7 +18634,7 @@
         <v>516</v>
       </c>
       <c r="B517" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C517">
         <v>3</v>
@@ -18673,7 +18666,7 @@
         <v>517</v>
       </c>
       <c r="B518" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C518">
         <v>4</v>
@@ -18705,7 +18698,7 @@
         <v>518</v>
       </c>
       <c r="B519" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C519">
         <v>4</v>
@@ -18737,7 +18730,7 @@
         <v>519</v>
       </c>
       <c r="B520" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C520">
         <v>4</v>
@@ -18769,7 +18762,7 @@
         <v>520</v>
       </c>
       <c r="B521" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C521">
         <v>1</v>
@@ -18801,7 +18794,7 @@
         <v>521</v>
       </c>
       <c r="B522" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C522">
         <v>2</v>
@@ -18833,7 +18826,7 @@
         <v>522</v>
       </c>
       <c r="B523" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C523">
         <v>1</v>
@@ -18865,7 +18858,7 @@
         <v>523</v>
       </c>
       <c r="B524" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C524">
         <v>4</v>
@@ -18897,7 +18890,7 @@
         <v>524</v>
       </c>
       <c r="B525" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C525">
         <v>4</v>
@@ -18929,7 +18922,7 @@
         <v>525</v>
       </c>
       <c r="B526" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C526">
         <v>1</v>
@@ -18961,7 +18954,7 @@
         <v>526</v>
       </c>
       <c r="B527" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C527">
         <v>2</v>
@@ -18993,7 +18986,7 @@
         <v>527</v>
       </c>
       <c r="B528" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C528">
         <v>3</v>
@@ -19025,7 +19018,7 @@
         <v>528</v>
       </c>
       <c r="B529" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C529">
         <v>2</v>
@@ -19057,7 +19050,7 @@
         <v>529</v>
       </c>
       <c r="B530" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C530">
         <v>2</v>
@@ -19089,7 +19082,7 @@
         <v>530</v>
       </c>
       <c r="B531" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C531">
         <v>3</v>
@@ -19121,7 +19114,7 @@
         <v>531</v>
       </c>
       <c r="B532" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C532">
         <v>3</v>
@@ -19153,7 +19146,7 @@
         <v>532</v>
       </c>
       <c r="B533" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C533">
         <v>4</v>
@@ -19185,7 +19178,7 @@
         <v>533</v>
       </c>
       <c r="B534" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C534">
         <v>5</v>
@@ -19217,7 +19210,7 @@
         <v>534</v>
       </c>
       <c r="B535" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C535">
         <v>2</v>
@@ -19249,7 +19242,7 @@
         <v>535</v>
       </c>
       <c r="B536" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C536">
         <v>3</v>
@@ -19281,7 +19274,7 @@
         <v>536</v>
       </c>
       <c r="B537" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C537">
         <v>2</v>
@@ -19313,7 +19306,7 @@
         <v>537</v>
       </c>
       <c r="B538" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C538">
         <v>3</v>
@@ -19345,7 +19338,7 @@
         <v>538</v>
       </c>
       <c r="B539" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C539">
         <v>1</v>
@@ -19377,7 +19370,7 @@
         <v>539</v>
       </c>
       <c r="B540" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C540">
         <v>3</v>
@@ -19409,7 +19402,7 @@
         <v>540</v>
       </c>
       <c r="B541" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="C541">
         <v>1</v>
@@ -19441,7 +19434,7 @@
         <v>541</v>
       </c>
       <c r="B542" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C542">
         <v>5</v>
@@ -19473,7 +19466,7 @@
         <v>542</v>
       </c>
       <c r="B543" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C543">
         <v>4</v>
@@ -19505,7 +19498,7 @@
         <v>543</v>
       </c>
       <c r="B544" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C544">
         <v>3</v>
@@ -19537,7 +19530,7 @@
         <v>544</v>
       </c>
       <c r="B545" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C545">
         <v>2</v>
@@ -19569,7 +19562,7 @@
         <v>545</v>
       </c>
       <c r="B546" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C546">
         <v>1</v>
@@ -19601,7 +19594,7 @@
         <v>546</v>
       </c>
       <c r="B547" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C547">
         <v>1</v>
@@ -19633,7 +19626,7 @@
         <v>547</v>
       </c>
       <c r="B548" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C548">
         <v>3</v>
@@ -19665,7 +19658,7 @@
         <v>548</v>
       </c>
       <c r="B549" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C549">
         <v>3</v>
@@ -19697,7 +19690,7 @@
         <v>549</v>
       </c>
       <c r="B550" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C550">
         <v>2</v>
@@ -19729,7 +19722,7 @@
         <v>550</v>
       </c>
       <c r="B551" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C551">
         <v>2</v>
@@ -19761,7 +19754,7 @@
         <v>551</v>
       </c>
       <c r="B552" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="C552">
         <v>2</v>
@@ -19793,7 +19786,7 @@
         <v>552</v>
       </c>
       <c r="B553" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C553">
         <v>4</v>
@@ -19825,7 +19818,7 @@
         <v>553</v>
       </c>
       <c r="B554" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C554">
         <v>2</v>
@@ -19857,7 +19850,7 @@
         <v>554</v>
       </c>
       <c r="B555" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C555">
         <v>1</v>
@@ -19889,7 +19882,7 @@
         <v>555</v>
       </c>
       <c r="B556" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C556">
         <v>3</v>
@@ -19921,7 +19914,7 @@
         <v>556</v>
       </c>
       <c r="B557" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C557">
         <v>1</v>
@@ -19953,7 +19946,7 @@
         <v>557</v>
       </c>
       <c r="B558" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C558">
         <v>1</v>
@@ -19985,7 +19978,7 @@
         <v>558</v>
       </c>
       <c r="B559" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C559">
         <v>1</v>
@@ -20017,7 +20010,7 @@
         <v>559</v>
       </c>
       <c r="B560" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C560">
         <v>2</v>
@@ -20049,7 +20042,7 @@
         <v>560</v>
       </c>
       <c r="B561" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C561">
         <v>1</v>
@@ -20113,7 +20106,7 @@
         <v>562</v>
       </c>
       <c r="B563" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C563">
         <v>3</v>
@@ -20145,7 +20138,7 @@
         <v>563</v>
       </c>
       <c r="B564" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C564">
         <v>2</v>

</xml_diff>